<commit_message>
Review lần hai phần Quản lí giao hàng
</commit_message>
<xml_diff>
--- a/BaoCao_Review/FD/[Team3][RV_FD]GiaoHang_KhuyenMai_BaoCaoThongKe.xlsx
+++ b/BaoCao_Review/FD/[Team3][RV_FD]GiaoHang_KhuyenMai_BaoCaoThongKe.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuga\Desktop\TH2014-1-PTUDHTTTHD-SaveMyLife-SML\BaoCao_Review\FD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester 7\PTUD HTTT\Project\TH2014-1-PTUDHTTTHD-SaveMyLife-SML\BaoCao_Review\FD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" tabRatio="475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" tabRatio="475"/>
   </bookViews>
   <sheets>
     <sheet name="Inspection" sheetId="9" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="345">
   <si>
     <t>Inform to:</t>
   </si>
@@ -1680,16 +1680,66 @@
     <t>23h</t>
   </si>
   <si>
-    <t>Review thiết kế chức năng</t>
-  </si>
-  <si>
     <t>Phạm Quốc Toàn</t>
+  </si>
+  <si>
+    <t>thiết kế chức năng hệ thống</t>
+  </si>
+  <si>
+    <t>thiết kế chức năng hệ thống sau review lần 1</t>
+  </si>
+  <si>
+    <t>Các class về phiếu ( đơn hàng,, đặt hàng...) không cần setID vì là thuộc tính tự tăng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xóa các phương thức setID trong các class liên quan đên đơn hàng( đơn giao hàng, đơn đặt hàng)
+</t>
+  </si>
+  <si>
+    <t>Class DonGiaoHang</t>
+  </si>
+  <si>
+    <t>Thiếu các phương thức về tìm kiếm theo các tiêu chí ( tình trạng, mã đơn…)</t>
+  </si>
+  <si>
+    <t>Thêm các phương thức về tìm kiếm theo các tiêu chí khác nhau ( tham khảo các usecase giao hàng để biết tiêu chí tìm kiếm)</t>
+  </si>
+  <si>
+    <t>TblDonGiaoHang</t>
+  </si>
+  <si>
+    <t>Sửa ID_DonHang thành ID_GiaoHang</t>
+  </si>
+  <si>
+    <t>Thuộc tính 1 không giống với class DonGiaoHang,</t>
+  </si>
+  <si>
+    <t>Thiếu thuộc tính TongTien</t>
+  </si>
+  <si>
+    <t>Thêm thuộc tính TongTien, kiểu dữ liệu Money</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Không cần mối quan hệ giữa NPP và  HoaDon ( vì có thể suy ra được từ quan hệ với DonDatHang) </t>
+  </si>
+  <si>
+    <t>Xóa mối quan hệ giữa NhaPhanPhoi va HoaDon, 
+xóa thuộc tính NPP ở bảng HoaDon</t>
+  </si>
+  <si>
+    <t>Thiếu Mô tả thuộc tính ID_GiaoHang ( DonGiaohang, CT_GiaoHang), ID_SanPham (CT_GiaoHang), ID_HoaDon (HoaDon)</t>
+  </si>
+  <si>
+    <t>Mô tả chi tiết</t>
+  </si>
+  <si>
+    <t>Thêm Mô tả thuộc tính ID_GiaoHang ( DonGiaohang, CT_GiaoHang), ID_SanPham (CT_GiaoHang), ID_HoaDon (HoaDon)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="10">
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="165" formatCode="0.00_ "/>
@@ -2519,7 +2569,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="603">
+  <cellXfs count="604">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3285,6 +3335,15 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="171" fontId="23" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -3326,15 +3385,6 @@
     <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="27" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -4352,19 +4402,22 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="標準 3" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="標準 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="標準_コードレビューに関するコメント_コードレビューチェックリストv0.22" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="標準_レビューチェックリスト_CD" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="標準_レビューチェックリスト_テスト仕様書" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="標準_レビューチェックリスト_テスト前" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="標準_レビューチェックリスト_テスト結果" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="標準_レビューチェックリスト_機能仕様書" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="標準_レビューチェックリスト_設計書" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="標準 2" xfId="1"/>
+    <cellStyle name="標準 3" xfId="9"/>
+    <cellStyle name="標準 4" xfId="10"/>
+    <cellStyle name="標準_コードレビューに関するコメント_コードレビューチェックリストv0.22" xfId="2"/>
+    <cellStyle name="標準_レビューチェックリスト_CD" xfId="3"/>
+    <cellStyle name="標準_レビューチェックリスト_テスト仕様書" xfId="5"/>
+    <cellStyle name="標準_レビューチェックリスト_テスト前" xfId="6"/>
+    <cellStyle name="標準_レビューチェックリスト_テスト結果" xfId="4"/>
+    <cellStyle name="標準_レビューチェックリスト_機能仕様書" xfId="7"/>
+    <cellStyle name="標準_レビューチェックリスト_設計書" xfId="8"/>
   </cellStyles>
   <dxfs count="98">
     <dxf>
@@ -18947,15 +19000,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AN82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A26" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36:P36"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A35" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41:V41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -18965,7 +19018,8 @@
     <col min="3" max="3" width="6.375" style="209" customWidth="1"/>
     <col min="4" max="4" width="10.125" style="209" customWidth="1"/>
     <col min="5" max="5" width="10.625" style="209" customWidth="1"/>
-    <col min="6" max="11" width="5.625" style="209" customWidth="1"/>
+    <col min="6" max="10" width="5.625" style="209" customWidth="1"/>
+    <col min="11" max="11" width="7.375" style="209" customWidth="1"/>
     <col min="12" max="12" width="6.375" style="209" customWidth="1"/>
     <col min="13" max="13" width="8.125" style="209" customWidth="1"/>
     <col min="14" max="14" width="8.375" style="209" customWidth="1"/>
@@ -19607,7 +19661,7 @@
       </c>
       <c r="C21" s="350"/>
       <c r="D21" s="351" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E21" s="351"/>
       <c r="F21" s="351"/>
@@ -19641,7 +19695,9 @@
         <v>27</v>
       </c>
       <c r="C22" s="350"/>
-      <c r="D22" s="351"/>
+      <c r="D22" s="351" t="s">
+        <v>329</v>
+      </c>
       <c r="E22" s="351"/>
       <c r="F22" s="351"/>
       <c r="G22" s="351"/>
@@ -19649,7 +19705,9 @@
       <c r="I22" s="351"/>
       <c r="J22" s="351"/>
       <c r="K22" s="351"/>
-      <c r="L22" s="351"/>
+      <c r="L22" s="351" t="s">
+        <v>296</v>
+      </c>
       <c r="M22" s="351"/>
       <c r="N22" s="351"/>
       <c r="O22" s="351"/>
@@ -19779,28 +19837,28 @@
       <c r="I26" s="334"/>
       <c r="J26" s="334"/>
       <c r="K26" s="334"/>
-      <c r="L26" s="271" t="s">
+      <c r="L26" s="274" t="s">
         <v>284</v>
       </c>
-      <c r="M26" s="272"/>
-      <c r="N26" s="266" t="s">
+      <c r="M26" s="275"/>
+      <c r="N26" s="269" t="s">
         <v>285</v>
       </c>
-      <c r="O26" s="266" t="s">
+      <c r="O26" s="269" t="s">
         <v>286</v>
       </c>
-      <c r="P26" s="266"/>
-      <c r="Q26" s="271" t="s">
+      <c r="P26" s="269"/>
+      <c r="Q26" s="274" t="s">
         <v>287</v>
       </c>
-      <c r="R26" s="275"/>
-      <c r="S26" s="275"/>
-      <c r="T26" s="275"/>
-      <c r="U26" s="275"/>
-      <c r="V26" s="272"/>
+      <c r="R26" s="278"/>
+      <c r="S26" s="278"/>
+      <c r="T26" s="278"/>
+      <c r="U26" s="278"/>
+      <c r="V26" s="275"/>
       <c r="W26" s="239"/>
-      <c r="X26" s="264"/>
-      <c r="Y26" s="265"/>
+      <c r="X26" s="267"/>
+      <c r="Y26" s="268"/>
     </row>
     <row r="27" spans="1:40" ht="41.25" customHeight="1">
       <c r="B27" s="281"/>
@@ -19817,20 +19875,20 @@
       <c r="I27" s="334"/>
       <c r="J27" s="334"/>
       <c r="K27" s="334"/>
-      <c r="L27" s="273"/>
-      <c r="M27" s="274"/>
-      <c r="N27" s="266"/>
-      <c r="O27" s="266"/>
-      <c r="P27" s="266"/>
-      <c r="Q27" s="273"/>
-      <c r="R27" s="276"/>
-      <c r="S27" s="276"/>
-      <c r="T27" s="276"/>
-      <c r="U27" s="276"/>
-      <c r="V27" s="274"/>
+      <c r="L27" s="276"/>
+      <c r="M27" s="277"/>
+      <c r="N27" s="269"/>
+      <c r="O27" s="269"/>
+      <c r="P27" s="269"/>
+      <c r="Q27" s="276"/>
+      <c r="R27" s="279"/>
+      <c r="S27" s="279"/>
+      <c r="T27" s="279"/>
+      <c r="U27" s="279"/>
+      <c r="V27" s="277"/>
       <c r="W27" s="239"/>
-      <c r="X27" s="264"/>
-      <c r="Y27" s="265"/>
+      <c r="X27" s="267"/>
+      <c r="Y27" s="268"/>
     </row>
     <row r="28" spans="1:40" ht="68.099999999999994" customHeight="1">
       <c r="B28" s="241">
@@ -19845,14 +19903,14 @@
       <c r="E28" s="244" t="s">
         <v>292</v>
       </c>
-      <c r="F28" s="267" t="s">
+      <c r="F28" s="270" t="s">
         <v>295</v>
       </c>
-      <c r="G28" s="268"/>
-      <c r="H28" s="268"/>
-      <c r="I28" s="268"/>
-      <c r="J28" s="268"/>
-      <c r="K28" s="268"/>
+      <c r="G28" s="271"/>
+      <c r="H28" s="271"/>
+      <c r="I28" s="271"/>
+      <c r="J28" s="271"/>
+      <c r="K28" s="271"/>
       <c r="L28" s="245" t="s">
         <v>254</v>
       </c>
@@ -19860,19 +19918,19 @@
         <v>307</v>
       </c>
       <c r="N28" s="239"/>
-      <c r="O28" s="269"/>
-      <c r="P28" s="270"/>
-      <c r="Q28" s="277" t="s">
+      <c r="O28" s="272"/>
+      <c r="P28" s="273"/>
+      <c r="Q28" s="264" t="s">
         <v>306</v>
       </c>
-      <c r="R28" s="278"/>
-      <c r="S28" s="278"/>
-      <c r="T28" s="278"/>
-      <c r="U28" s="278"/>
-      <c r="V28" s="279"/>
+      <c r="R28" s="265"/>
+      <c r="S28" s="265"/>
+      <c r="T28" s="265"/>
+      <c r="U28" s="265"/>
+      <c r="V28" s="266"/>
       <c r="W28" s="239"/>
-      <c r="X28" s="264"/>
-      <c r="Y28" s="265"/>
+      <c r="X28" s="267"/>
+      <c r="Y28" s="268"/>
     </row>
     <row r="29" spans="1:40" ht="84" customHeight="1">
       <c r="B29" s="241">
@@ -19887,14 +19945,14 @@
       <c r="E29" s="244" t="s">
         <v>292</v>
       </c>
-      <c r="F29" s="267" t="s">
+      <c r="F29" s="270" t="s">
         <v>299</v>
       </c>
-      <c r="G29" s="268"/>
-      <c r="H29" s="268"/>
-      <c r="I29" s="268"/>
-      <c r="J29" s="268"/>
-      <c r="K29" s="268"/>
+      <c r="G29" s="271"/>
+      <c r="H29" s="271"/>
+      <c r="I29" s="271"/>
+      <c r="J29" s="271"/>
+      <c r="K29" s="271"/>
       <c r="L29" s="245" t="s">
         <v>254</v>
       </c>
@@ -19902,19 +19960,19 @@
         <v>255</v>
       </c>
       <c r="N29" s="239"/>
-      <c r="O29" s="269"/>
-      <c r="P29" s="270"/>
-      <c r="Q29" s="277" t="s">
+      <c r="O29" s="272"/>
+      <c r="P29" s="273"/>
+      <c r="Q29" s="264" t="s">
         <v>305</v>
       </c>
-      <c r="R29" s="278"/>
-      <c r="S29" s="278"/>
-      <c r="T29" s="278"/>
-      <c r="U29" s="278"/>
-      <c r="V29" s="279"/>
+      <c r="R29" s="265"/>
+      <c r="S29" s="265"/>
+      <c r="T29" s="265"/>
+      <c r="U29" s="265"/>
+      <c r="V29" s="266"/>
       <c r="W29" s="239"/>
-      <c r="X29" s="264"/>
-      <c r="Y29" s="265"/>
+      <c r="X29" s="267"/>
+      <c r="Y29" s="268"/>
     </row>
     <row r="30" spans="1:40" ht="69" customHeight="1">
       <c r="B30" s="241">
@@ -19929,14 +19987,14 @@
       <c r="E30" s="244" t="s">
         <v>292</v>
       </c>
-      <c r="F30" s="267" t="s">
+      <c r="F30" s="270" t="s">
         <v>300</v>
       </c>
-      <c r="G30" s="268"/>
-      <c r="H30" s="268"/>
-      <c r="I30" s="268"/>
-      <c r="J30" s="268"/>
-      <c r="K30" s="268"/>
+      <c r="G30" s="271"/>
+      <c r="H30" s="271"/>
+      <c r="I30" s="271"/>
+      <c r="J30" s="271"/>
+      <c r="K30" s="271"/>
       <c r="L30" s="245" t="s">
         <v>254</v>
       </c>
@@ -19944,19 +20002,19 @@
         <v>255</v>
       </c>
       <c r="N30" s="239"/>
-      <c r="O30" s="269"/>
-      <c r="P30" s="270"/>
-      <c r="Q30" s="277" t="s">
+      <c r="O30" s="272"/>
+      <c r="P30" s="273"/>
+      <c r="Q30" s="264" t="s">
         <v>304</v>
       </c>
-      <c r="R30" s="278"/>
-      <c r="S30" s="278"/>
-      <c r="T30" s="278"/>
-      <c r="U30" s="278"/>
-      <c r="V30" s="279"/>
+      <c r="R30" s="265"/>
+      <c r="S30" s="265"/>
+      <c r="T30" s="265"/>
+      <c r="U30" s="265"/>
+      <c r="V30" s="266"/>
       <c r="W30" s="239"/>
-      <c r="X30" s="264"/>
-      <c r="Y30" s="265"/>
+      <c r="X30" s="267"/>
+      <c r="Y30" s="268"/>
     </row>
     <row r="31" spans="1:40" ht="42" customHeight="1">
       <c r="B31" s="241">
@@ -19971,14 +20029,14 @@
       <c r="E31" s="244" t="s">
         <v>292</v>
       </c>
-      <c r="F31" s="267" t="s">
+      <c r="F31" s="270" t="s">
         <v>301</v>
       </c>
-      <c r="G31" s="268"/>
-      <c r="H31" s="268"/>
-      <c r="I31" s="268"/>
-      <c r="J31" s="268"/>
-      <c r="K31" s="268"/>
+      <c r="G31" s="271"/>
+      <c r="H31" s="271"/>
+      <c r="I31" s="271"/>
+      <c r="J31" s="271"/>
+      <c r="K31" s="271"/>
       <c r="L31" s="245" t="s">
         <v>254</v>
       </c>
@@ -19986,23 +20044,23 @@
         <v>303</v>
       </c>
       <c r="N31" s="239" t="s">
-        <v>328</v>
-      </c>
-      <c r="O31" s="269">
+        <v>327</v>
+      </c>
+      <c r="O31" s="272">
         <v>43036</v>
       </c>
-      <c r="P31" s="270"/>
-      <c r="Q31" s="277" t="s">
+      <c r="P31" s="273"/>
+      <c r="Q31" s="264" t="s">
         <v>302</v>
       </c>
-      <c r="R31" s="278"/>
-      <c r="S31" s="278"/>
-      <c r="T31" s="278"/>
-      <c r="U31" s="278"/>
-      <c r="V31" s="279"/>
+      <c r="R31" s="265"/>
+      <c r="S31" s="265"/>
+      <c r="T31" s="265"/>
+      <c r="U31" s="265"/>
+      <c r="V31" s="266"/>
       <c r="W31" s="239"/>
-      <c r="X31" s="264"/>
-      <c r="Y31" s="265"/>
+      <c r="X31" s="267"/>
+      <c r="Y31" s="268"/>
     </row>
     <row r="32" spans="1:40" ht="42" customHeight="1">
       <c r="B32" s="241">
@@ -20017,14 +20075,14 @@
       <c r="E32" s="244" t="s">
         <v>310</v>
       </c>
-      <c r="F32" s="267" t="s">
+      <c r="F32" s="270" t="s">
         <v>311</v>
       </c>
-      <c r="G32" s="268"/>
-      <c r="H32" s="268"/>
-      <c r="I32" s="268"/>
-      <c r="J32" s="268"/>
-      <c r="K32" s="268"/>
+      <c r="G32" s="271"/>
+      <c r="H32" s="271"/>
+      <c r="I32" s="271"/>
+      <c r="J32" s="271"/>
+      <c r="K32" s="271"/>
       <c r="L32" s="245" t="s">
         <v>254</v>
       </c>
@@ -20032,23 +20090,23 @@
         <v>303</v>
       </c>
       <c r="N32" s="239" t="s">
-        <v>328</v>
-      </c>
-      <c r="O32" s="269">
+        <v>327</v>
+      </c>
+      <c r="O32" s="272">
         <v>43036</v>
       </c>
-      <c r="P32" s="270"/>
-      <c r="Q32" s="277" t="s">
+      <c r="P32" s="273"/>
+      <c r="Q32" s="264" t="s">
         <v>312</v>
       </c>
-      <c r="R32" s="278"/>
-      <c r="S32" s="278"/>
-      <c r="T32" s="278"/>
-      <c r="U32" s="278"/>
-      <c r="V32" s="279"/>
+      <c r="R32" s="265"/>
+      <c r="S32" s="265"/>
+      <c r="T32" s="265"/>
+      <c r="U32" s="265"/>
+      <c r="V32" s="266"/>
       <c r="W32" s="239"/>
-      <c r="X32" s="264"/>
-      <c r="Y32" s="265"/>
+      <c r="X32" s="267"/>
+      <c r="Y32" s="268"/>
     </row>
     <row r="33" spans="1:26" ht="42" customHeight="1">
       <c r="B33" s="241">
@@ -20063,14 +20121,14 @@
       <c r="E33" s="244" t="s">
         <v>310</v>
       </c>
-      <c r="F33" s="267" t="s">
+      <c r="F33" s="270" t="s">
         <v>313</v>
       </c>
-      <c r="G33" s="268"/>
-      <c r="H33" s="268"/>
-      <c r="I33" s="268"/>
-      <c r="J33" s="268"/>
-      <c r="K33" s="268"/>
+      <c r="G33" s="271"/>
+      <c r="H33" s="271"/>
+      <c r="I33" s="271"/>
+      <c r="J33" s="271"/>
+      <c r="K33" s="271"/>
       <c r="L33" s="245" t="s">
         <v>254</v>
       </c>
@@ -20078,23 +20136,23 @@
         <v>303</v>
       </c>
       <c r="N33" s="239" t="s">
-        <v>328</v>
-      </c>
-      <c r="O33" s="269">
+        <v>327</v>
+      </c>
+      <c r="O33" s="272">
         <v>43036</v>
       </c>
-      <c r="P33" s="270"/>
-      <c r="Q33" s="277" t="s">
+      <c r="P33" s="273"/>
+      <c r="Q33" s="264" t="s">
         <v>314</v>
       </c>
-      <c r="R33" s="278"/>
-      <c r="S33" s="278"/>
-      <c r="T33" s="278"/>
-      <c r="U33" s="278"/>
-      <c r="V33" s="279"/>
+      <c r="R33" s="265"/>
+      <c r="S33" s="265"/>
+      <c r="T33" s="265"/>
+      <c r="U33" s="265"/>
+      <c r="V33" s="266"/>
       <c r="W33" s="239"/>
-      <c r="X33" s="264"/>
-      <c r="Y33" s="265"/>
+      <c r="X33" s="267"/>
+      <c r="Y33" s="268"/>
     </row>
     <row r="34" spans="1:26" ht="42" customHeight="1">
       <c r="B34" s="241">
@@ -20109,14 +20167,14 @@
       <c r="E34" s="244" t="s">
         <v>310</v>
       </c>
-      <c r="F34" s="267" t="s">
+      <c r="F34" s="270" t="s">
         <v>315</v>
       </c>
-      <c r="G34" s="268"/>
-      <c r="H34" s="268"/>
-      <c r="I34" s="268"/>
-      <c r="J34" s="268"/>
-      <c r="K34" s="268"/>
+      <c r="G34" s="271"/>
+      <c r="H34" s="271"/>
+      <c r="I34" s="271"/>
+      <c r="J34" s="271"/>
+      <c r="K34" s="271"/>
       <c r="L34" s="245" t="s">
         <v>254</v>
       </c>
@@ -20124,23 +20182,23 @@
         <v>255</v>
       </c>
       <c r="N34" s="239" t="s">
-        <v>328</v>
-      </c>
-      <c r="O34" s="269">
+        <v>327</v>
+      </c>
+      <c r="O34" s="272">
         <v>43036</v>
       </c>
-      <c r="P34" s="270"/>
-      <c r="Q34" s="277" t="s">
+      <c r="P34" s="273"/>
+      <c r="Q34" s="264" t="s">
         <v>316</v>
       </c>
-      <c r="R34" s="278"/>
-      <c r="S34" s="278"/>
-      <c r="T34" s="278"/>
-      <c r="U34" s="278"/>
-      <c r="V34" s="279"/>
+      <c r="R34" s="265"/>
+      <c r="S34" s="265"/>
+      <c r="T34" s="265"/>
+      <c r="U34" s="265"/>
+      <c r="V34" s="266"/>
       <c r="W34" s="239"/>
-      <c r="X34" s="264"/>
-      <c r="Y34" s="265"/>
+      <c r="X34" s="267"/>
+      <c r="Y34" s="268"/>
     </row>
     <row r="35" spans="1:26" ht="42" customHeight="1">
       <c r="B35" s="241">
@@ -20155,14 +20213,14 @@
       <c r="E35" s="244" t="s">
         <v>310</v>
       </c>
-      <c r="F35" s="267" t="s">
+      <c r="F35" s="270" t="s">
         <v>318</v>
       </c>
-      <c r="G35" s="268"/>
-      <c r="H35" s="268"/>
-      <c r="I35" s="268"/>
-      <c r="J35" s="268"/>
-      <c r="K35" s="268"/>
+      <c r="G35" s="271"/>
+      <c r="H35" s="271"/>
+      <c r="I35" s="271"/>
+      <c r="J35" s="271"/>
+      <c r="K35" s="271"/>
       <c r="L35" s="245" t="s">
         <v>254</v>
       </c>
@@ -20170,23 +20228,23 @@
         <v>303</v>
       </c>
       <c r="N35" s="239" t="s">
-        <v>328</v>
-      </c>
-      <c r="O35" s="269">
+        <v>327</v>
+      </c>
+      <c r="O35" s="272">
         <v>43036</v>
       </c>
-      <c r="P35" s="270"/>
-      <c r="Q35" s="277" t="s">
+      <c r="P35" s="273"/>
+      <c r="Q35" s="264" t="s">
         <v>319</v>
       </c>
-      <c r="R35" s="278"/>
-      <c r="S35" s="278"/>
-      <c r="T35" s="278"/>
-      <c r="U35" s="278"/>
-      <c r="V35" s="279"/>
+      <c r="R35" s="265"/>
+      <c r="S35" s="265"/>
+      <c r="T35" s="265"/>
+      <c r="U35" s="265"/>
+      <c r="V35" s="266"/>
       <c r="W35" s="239"/>
-      <c r="X35" s="264"/>
-      <c r="Y35" s="265"/>
+      <c r="X35" s="267"/>
+      <c r="Y35" s="268"/>
     </row>
     <row r="36" spans="1:26" ht="42" customHeight="1">
       <c r="A36" s="233"/>
@@ -20194,34 +20252,42 @@
         <v>9</v>
       </c>
       <c r="C36" s="242" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="243"/>
-      <c r="E36" s="244"/>
-      <c r="F36" s="267"/>
-      <c r="G36" s="268"/>
-      <c r="H36" s="268"/>
-      <c r="I36" s="268"/>
-      <c r="J36" s="268"/>
-      <c r="K36" s="268"/>
+        <v>27</v>
+      </c>
+      <c r="D36" s="243" t="s">
+        <v>309</v>
+      </c>
+      <c r="E36" s="244" t="s">
+        <v>310</v>
+      </c>
+      <c r="F36" s="270" t="s">
+        <v>330</v>
+      </c>
+      <c r="G36" s="271"/>
+      <c r="H36" s="271"/>
+      <c r="I36" s="271"/>
+      <c r="J36" s="271"/>
+      <c r="K36" s="271"/>
       <c r="L36" s="245" t="s">
-        <v>60</v>
+        <v>254</v>
       </c>
       <c r="M36" s="246" t="s">
-        <v>60</v>
+        <v>303</v>
       </c>
       <c r="N36" s="239"/>
-      <c r="O36" s="269"/>
-      <c r="P36" s="270"/>
-      <c r="Q36" s="247"/>
-      <c r="R36" s="248"/>
-      <c r="S36" s="248"/>
-      <c r="T36" s="248"/>
-      <c r="U36" s="248"/>
-      <c r="V36" s="249"/>
+      <c r="O36" s="272"/>
+      <c r="P36" s="273"/>
+      <c r="Q36" s="264" t="s">
+        <v>331</v>
+      </c>
+      <c r="R36" s="265"/>
+      <c r="S36" s="265"/>
+      <c r="T36" s="265"/>
+      <c r="U36" s="265"/>
+      <c r="V36" s="266"/>
       <c r="W36" s="239"/>
-      <c r="X36" s="264"/>
-      <c r="Y36" s="265"/>
+      <c r="X36" s="267"/>
+      <c r="Y36" s="268"/>
       <c r="Z36" s="213"/>
     </row>
     <row r="37" spans="1:26" ht="42" customHeight="1">
@@ -20230,34 +20296,42 @@
         <v>10</v>
       </c>
       <c r="C37" s="242" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="243"/>
-      <c r="E37" s="244"/>
-      <c r="F37" s="267"/>
-      <c r="G37" s="268"/>
-      <c r="H37" s="268"/>
-      <c r="I37" s="268"/>
-      <c r="J37" s="268"/>
-      <c r="K37" s="268"/>
+        <v>27</v>
+      </c>
+      <c r="D37" s="243" t="s">
+        <v>332</v>
+      </c>
+      <c r="E37" s="244" t="s">
+        <v>310</v>
+      </c>
+      <c r="F37" s="270" t="s">
+        <v>333</v>
+      </c>
+      <c r="G37" s="271"/>
+      <c r="H37" s="271"/>
+      <c r="I37" s="271"/>
+      <c r="J37" s="271"/>
+      <c r="K37" s="271"/>
       <c r="L37" s="245" t="s">
-        <v>60</v>
+        <v>254</v>
       </c>
       <c r="M37" s="246" t="s">
-        <v>60</v>
+        <v>255</v>
       </c>
       <c r="N37" s="239"/>
-      <c r="O37" s="269"/>
-      <c r="P37" s="270"/>
-      <c r="Q37" s="247"/>
-      <c r="R37" s="248"/>
-      <c r="S37" s="248"/>
-      <c r="T37" s="248"/>
-      <c r="U37" s="248"/>
-      <c r="V37" s="249"/>
+      <c r="O37" s="272"/>
+      <c r="P37" s="273"/>
+      <c r="Q37" s="264" t="s">
+        <v>334</v>
+      </c>
+      <c r="R37" s="265"/>
+      <c r="S37" s="265"/>
+      <c r="T37" s="265"/>
+      <c r="U37" s="265"/>
+      <c r="V37" s="266"/>
       <c r="W37" s="239"/>
-      <c r="X37" s="264"/>
-      <c r="Y37" s="265"/>
+      <c r="X37" s="267"/>
+      <c r="Y37" s="268"/>
       <c r="Z37" s="213"/>
     </row>
     <row r="38" spans="1:26" ht="42" customHeight="1">
@@ -20266,34 +20340,42 @@
         <v>11</v>
       </c>
       <c r="C38" s="242" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" s="243"/>
-      <c r="E38" s="244"/>
-      <c r="F38" s="267"/>
-      <c r="G38" s="268"/>
-      <c r="H38" s="268"/>
-      <c r="I38" s="268"/>
-      <c r="J38" s="268"/>
-      <c r="K38" s="268"/>
+        <v>27</v>
+      </c>
+      <c r="D38" s="243" t="s">
+        <v>335</v>
+      </c>
+      <c r="E38" s="244" t="s">
+        <v>310</v>
+      </c>
+      <c r="F38" s="270" t="s">
+        <v>337</v>
+      </c>
+      <c r="G38" s="271"/>
+      <c r="H38" s="271"/>
+      <c r="I38" s="271"/>
+      <c r="J38" s="271"/>
+      <c r="K38" s="271"/>
       <c r="L38" s="245" t="s">
-        <v>60</v>
+        <v>254</v>
       </c>
       <c r="M38" s="246" t="s">
-        <v>60</v>
+        <v>303</v>
       </c>
       <c r="N38" s="239"/>
-      <c r="O38" s="269"/>
-      <c r="P38" s="270"/>
-      <c r="Q38" s="247"/>
-      <c r="R38" s="248"/>
-      <c r="S38" s="248"/>
-      <c r="T38" s="248"/>
-      <c r="U38" s="248"/>
-      <c r="V38" s="249"/>
+      <c r="O38" s="272"/>
+      <c r="P38" s="273"/>
+      <c r="Q38" s="264" t="s">
+        <v>336</v>
+      </c>
+      <c r="R38" s="265"/>
+      <c r="S38" s="265"/>
+      <c r="T38" s="265"/>
+      <c r="U38" s="265"/>
+      <c r="V38" s="266"/>
       <c r="W38" s="239"/>
-      <c r="X38" s="264"/>
-      <c r="Y38" s="265"/>
+      <c r="X38" s="267"/>
+      <c r="Y38" s="268"/>
       <c r="Z38" s="213"/>
     </row>
     <row r="39" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
@@ -20302,34 +20384,42 @@
         <v>12</v>
       </c>
       <c r="C39" s="242" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" s="243"/>
-      <c r="E39" s="244"/>
-      <c r="F39" s="267"/>
-      <c r="G39" s="268"/>
-      <c r="H39" s="268"/>
-      <c r="I39" s="268"/>
-      <c r="J39" s="268"/>
-      <c r="K39" s="268"/>
+        <v>27</v>
+      </c>
+      <c r="D39" s="243" t="s">
+        <v>335</v>
+      </c>
+      <c r="E39" s="244" t="s">
+        <v>310</v>
+      </c>
+      <c r="F39" s="270" t="s">
+        <v>338</v>
+      </c>
+      <c r="G39" s="271"/>
+      <c r="H39" s="271"/>
+      <c r="I39" s="271"/>
+      <c r="J39" s="271"/>
+      <c r="K39" s="271"/>
       <c r="L39" s="245" t="s">
-        <v>60</v>
+        <v>254</v>
       </c>
       <c r="M39" s="246" t="s">
-        <v>60</v>
+        <v>255</v>
       </c>
       <c r="N39" s="239"/>
-      <c r="O39" s="269"/>
-      <c r="P39" s="270"/>
-      <c r="Q39" s="247"/>
-      <c r="R39" s="248"/>
-      <c r="S39" s="248"/>
-      <c r="T39" s="248"/>
-      <c r="U39" s="248"/>
-      <c r="V39" s="249"/>
+      <c r="O39" s="272"/>
+      <c r="P39" s="273"/>
+      <c r="Q39" s="264" t="s">
+        <v>339</v>
+      </c>
+      <c r="R39" s="265"/>
+      <c r="S39" s="265"/>
+      <c r="T39" s="265"/>
+      <c r="U39" s="265"/>
+      <c r="V39" s="266"/>
       <c r="W39" s="239"/>
-      <c r="X39" s="264"/>
-      <c r="Y39" s="265"/>
+      <c r="X39" s="267"/>
+      <c r="Y39" s="268"/>
     </row>
     <row r="40" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
       <c r="A40" s="250"/>
@@ -20337,34 +20427,42 @@
         <v>13</v>
       </c>
       <c r="C40" s="242" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" s="243"/>
-      <c r="E40" s="244"/>
-      <c r="F40" s="267"/>
-      <c r="G40" s="268"/>
-      <c r="H40" s="268"/>
-      <c r="I40" s="268"/>
-      <c r="J40" s="268"/>
-      <c r="K40" s="268"/>
+        <v>27</v>
+      </c>
+      <c r="D40" s="603" t="s">
+        <v>309</v>
+      </c>
+      <c r="E40" s="244" t="s">
+        <v>310</v>
+      </c>
+      <c r="F40" s="270" t="s">
+        <v>340</v>
+      </c>
+      <c r="G40" s="271"/>
+      <c r="H40" s="271"/>
+      <c r="I40" s="271"/>
+      <c r="J40" s="271"/>
+      <c r="K40" s="271"/>
       <c r="L40" s="245" t="s">
-        <v>60</v>
+        <v>254</v>
       </c>
       <c r="M40" s="246" t="s">
-        <v>60</v>
+        <v>303</v>
       </c>
       <c r="N40" s="239"/>
-      <c r="O40" s="269"/>
-      <c r="P40" s="270"/>
-      <c r="Q40" s="247"/>
-      <c r="R40" s="248"/>
-      <c r="S40" s="248"/>
-      <c r="T40" s="248"/>
-      <c r="U40" s="248"/>
-      <c r="V40" s="249"/>
+      <c r="O40" s="272"/>
+      <c r="P40" s="273"/>
+      <c r="Q40" s="264" t="s">
+        <v>341</v>
+      </c>
+      <c r="R40" s="265"/>
+      <c r="S40" s="265"/>
+      <c r="T40" s="265"/>
+      <c r="U40" s="265"/>
+      <c r="V40" s="266"/>
       <c r="W40" s="239"/>
-      <c r="X40" s="264"/>
-      <c r="Y40" s="265"/>
+      <c r="X40" s="267"/>
+      <c r="Y40" s="268"/>
     </row>
     <row r="41" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
       <c r="A41" s="250"/>
@@ -20372,34 +20470,42 @@
         <v>14</v>
       </c>
       <c r="C41" s="242" t="s">
-        <v>60</v>
-      </c>
-      <c r="D41" s="243"/>
-      <c r="E41" s="244"/>
-      <c r="F41" s="267"/>
-      <c r="G41" s="268"/>
-      <c r="H41" s="268"/>
-      <c r="I41" s="268"/>
-      <c r="J41" s="268"/>
-      <c r="K41" s="268"/>
+        <v>27</v>
+      </c>
+      <c r="D41" s="243" t="s">
+        <v>343</v>
+      </c>
+      <c r="E41" s="244" t="s">
+        <v>310</v>
+      </c>
+      <c r="F41" s="270" t="s">
+        <v>342</v>
+      </c>
+      <c r="G41" s="271"/>
+      <c r="H41" s="271"/>
+      <c r="I41" s="271"/>
+      <c r="J41" s="271"/>
+      <c r="K41" s="271"/>
       <c r="L41" s="245" t="s">
-        <v>60</v>
+        <v>254</v>
       </c>
       <c r="M41" s="246" t="s">
-        <v>60</v>
+        <v>255</v>
       </c>
       <c r="N41" s="239"/>
-      <c r="O41" s="269"/>
-      <c r="P41" s="270"/>
-      <c r="Q41" s="247"/>
-      <c r="R41" s="248"/>
-      <c r="S41" s="248"/>
-      <c r="T41" s="248"/>
-      <c r="U41" s="248"/>
-      <c r="V41" s="249"/>
+      <c r="O41" s="272"/>
+      <c r="P41" s="273"/>
+      <c r="Q41" s="270" t="s">
+        <v>344</v>
+      </c>
+      <c r="R41" s="271"/>
+      <c r="S41" s="271"/>
+      <c r="T41" s="271"/>
+      <c r="U41" s="271"/>
+      <c r="V41" s="271"/>
       <c r="W41" s="239"/>
-      <c r="X41" s="264"/>
-      <c r="Y41" s="265"/>
+      <c r="X41" s="267"/>
+      <c r="Y41" s="268"/>
     </row>
     <row r="42" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
       <c r="A42" s="250"/>
@@ -20411,12 +20517,12 @@
       </c>
       <c r="D42" s="243"/>
       <c r="E42" s="244"/>
-      <c r="F42" s="267"/>
-      <c r="G42" s="268"/>
-      <c r="H42" s="268"/>
-      <c r="I42" s="268"/>
-      <c r="J42" s="268"/>
-      <c r="K42" s="268"/>
+      <c r="F42" s="270"/>
+      <c r="G42" s="271"/>
+      <c r="H42" s="271"/>
+      <c r="I42" s="271"/>
+      <c r="J42" s="271"/>
+      <c r="K42" s="271"/>
       <c r="L42" s="245" t="s">
         <v>60</v>
       </c>
@@ -20424,8 +20530,8 @@
         <v>60</v>
       </c>
       <c r="N42" s="239"/>
-      <c r="O42" s="269"/>
-      <c r="P42" s="270"/>
+      <c r="O42" s="272"/>
+      <c r="P42" s="273"/>
       <c r="Q42" s="247"/>
       <c r="R42" s="248"/>
       <c r="S42" s="248"/>
@@ -20433,8 +20539,8 @@
       <c r="U42" s="248"/>
       <c r="V42" s="249"/>
       <c r="W42" s="239"/>
-      <c r="X42" s="264"/>
-      <c r="Y42" s="265"/>
+      <c r="X42" s="267"/>
+      <c r="Y42" s="268"/>
     </row>
     <row r="43" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
       <c r="A43" s="250"/>
@@ -20446,12 +20552,12 @@
       </c>
       <c r="D43" s="243"/>
       <c r="E43" s="244"/>
-      <c r="F43" s="267"/>
-      <c r="G43" s="268"/>
-      <c r="H43" s="268"/>
-      <c r="I43" s="268"/>
-      <c r="J43" s="268"/>
-      <c r="K43" s="268"/>
+      <c r="F43" s="270"/>
+      <c r="G43" s="271"/>
+      <c r="H43" s="271"/>
+      <c r="I43" s="271"/>
+      <c r="J43" s="271"/>
+      <c r="K43" s="271"/>
       <c r="L43" s="245" t="s">
         <v>60</v>
       </c>
@@ -20459,8 +20565,8 @@
         <v>60</v>
       </c>
       <c r="N43" s="239"/>
-      <c r="O43" s="269"/>
-      <c r="P43" s="270"/>
+      <c r="O43" s="272"/>
+      <c r="P43" s="273"/>
       <c r="Q43" s="247"/>
       <c r="R43" s="248"/>
       <c r="S43" s="248"/>
@@ -20468,8 +20574,8 @@
       <c r="U43" s="248"/>
       <c r="V43" s="249"/>
       <c r="W43" s="239"/>
-      <c r="X43" s="264"/>
-      <c r="Y43" s="265"/>
+      <c r="X43" s="267"/>
+      <c r="Y43" s="268"/>
     </row>
     <row r="44" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
       <c r="A44" s="250"/>
@@ -20481,12 +20587,12 @@
       </c>
       <c r="D44" s="243"/>
       <c r="E44" s="244"/>
-      <c r="F44" s="267"/>
-      <c r="G44" s="268"/>
-      <c r="H44" s="268"/>
-      <c r="I44" s="268"/>
-      <c r="J44" s="268"/>
-      <c r="K44" s="268"/>
+      <c r="F44" s="270"/>
+      <c r="G44" s="271"/>
+      <c r="H44" s="271"/>
+      <c r="I44" s="271"/>
+      <c r="J44" s="271"/>
+      <c r="K44" s="271"/>
       <c r="L44" s="245" t="s">
         <v>60</v>
       </c>
@@ -20494,8 +20600,8 @@
         <v>60</v>
       </c>
       <c r="N44" s="239"/>
-      <c r="O44" s="269"/>
-      <c r="P44" s="270"/>
+      <c r="O44" s="272"/>
+      <c r="P44" s="273"/>
       <c r="Q44" s="247"/>
       <c r="R44" s="248"/>
       <c r="S44" s="248"/>
@@ -20503,8 +20609,8 @@
       <c r="U44" s="248"/>
       <c r="V44" s="249"/>
       <c r="W44" s="239"/>
-      <c r="X44" s="264"/>
-      <c r="Y44" s="265"/>
+      <c r="X44" s="267"/>
+      <c r="Y44" s="268"/>
     </row>
     <row r="45" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
       <c r="A45" s="250"/>
@@ -20516,12 +20622,12 @@
       </c>
       <c r="D45" s="243"/>
       <c r="E45" s="244"/>
-      <c r="F45" s="267"/>
-      <c r="G45" s="268"/>
-      <c r="H45" s="268"/>
-      <c r="I45" s="268"/>
-      <c r="J45" s="268"/>
-      <c r="K45" s="268"/>
+      <c r="F45" s="270"/>
+      <c r="G45" s="271"/>
+      <c r="H45" s="271"/>
+      <c r="I45" s="271"/>
+      <c r="J45" s="271"/>
+      <c r="K45" s="271"/>
       <c r="L45" s="245" t="s">
         <v>60</v>
       </c>
@@ -20529,8 +20635,8 @@
         <v>60</v>
       </c>
       <c r="N45" s="239"/>
-      <c r="O45" s="269"/>
-      <c r="P45" s="270"/>
+      <c r="O45" s="272"/>
+      <c r="P45" s="273"/>
       <c r="Q45" s="247"/>
       <c r="R45" s="248"/>
       <c r="S45" s="248"/>
@@ -20538,8 +20644,8 @@
       <c r="U45" s="248"/>
       <c r="V45" s="249"/>
       <c r="W45" s="239"/>
-      <c r="X45" s="264"/>
-      <c r="Y45" s="265"/>
+      <c r="X45" s="267"/>
+      <c r="Y45" s="268"/>
     </row>
     <row r="46" spans="1:26" ht="42" customHeight="1">
       <c r="B46" s="241">
@@ -20550,12 +20656,12 @@
       </c>
       <c r="D46" s="243"/>
       <c r="E46" s="244"/>
-      <c r="F46" s="267"/>
-      <c r="G46" s="268"/>
-      <c r="H46" s="268"/>
-      <c r="I46" s="268"/>
-      <c r="J46" s="268"/>
-      <c r="K46" s="268"/>
+      <c r="F46" s="270"/>
+      <c r="G46" s="271"/>
+      <c r="H46" s="271"/>
+      <c r="I46" s="271"/>
+      <c r="J46" s="271"/>
+      <c r="K46" s="271"/>
       <c r="L46" s="245" t="s">
         <v>60</v>
       </c>
@@ -20563,8 +20669,8 @@
         <v>60</v>
       </c>
       <c r="N46" s="239"/>
-      <c r="O46" s="269"/>
-      <c r="P46" s="270"/>
+      <c r="O46" s="272"/>
+      <c r="P46" s="273"/>
       <c r="Q46" s="247"/>
       <c r="R46" s="248"/>
       <c r="S46" s="248"/>
@@ -20572,8 +20678,8 @@
       <c r="U46" s="248"/>
       <c r="V46" s="249"/>
       <c r="W46" s="239"/>
-      <c r="X46" s="264"/>
-      <c r="Y46" s="265"/>
+      <c r="X46" s="267"/>
+      <c r="Y46" s="268"/>
     </row>
     <row r="47" spans="1:26" ht="42" customHeight="1">
       <c r="B47" s="241">
@@ -20584,12 +20690,12 @@
       </c>
       <c r="D47" s="243"/>
       <c r="E47" s="244"/>
-      <c r="F47" s="267"/>
-      <c r="G47" s="268"/>
-      <c r="H47" s="268"/>
-      <c r="I47" s="268"/>
-      <c r="J47" s="268"/>
-      <c r="K47" s="268"/>
+      <c r="F47" s="270"/>
+      <c r="G47" s="271"/>
+      <c r="H47" s="271"/>
+      <c r="I47" s="271"/>
+      <c r="J47" s="271"/>
+      <c r="K47" s="271"/>
       <c r="L47" s="245" t="s">
         <v>60</v>
       </c>
@@ -20597,8 +20703,8 @@
         <v>60</v>
       </c>
       <c r="N47" s="239"/>
-      <c r="O47" s="269"/>
-      <c r="P47" s="270"/>
+      <c r="O47" s="272"/>
+      <c r="P47" s="273"/>
       <c r="Q47" s="247"/>
       <c r="R47" s="248"/>
       <c r="S47" s="248"/>
@@ -20606,8 +20712,8 @@
       <c r="U47" s="248"/>
       <c r="V47" s="249"/>
       <c r="W47" s="239"/>
-      <c r="X47" s="264"/>
-      <c r="Y47" s="265"/>
+      <c r="X47" s="267"/>
+      <c r="Y47" s="268"/>
     </row>
     <row r="48" spans="1:26" ht="42" customHeight="1">
       <c r="B48" s="241">
@@ -20618,12 +20724,12 @@
       </c>
       <c r="D48" s="243"/>
       <c r="E48" s="244"/>
-      <c r="F48" s="267"/>
-      <c r="G48" s="268"/>
-      <c r="H48" s="268"/>
-      <c r="I48" s="268"/>
-      <c r="J48" s="268"/>
-      <c r="K48" s="268"/>
+      <c r="F48" s="270"/>
+      <c r="G48" s="271"/>
+      <c r="H48" s="271"/>
+      <c r="I48" s="271"/>
+      <c r="J48" s="271"/>
+      <c r="K48" s="271"/>
       <c r="L48" s="245" t="s">
         <v>60</v>
       </c>
@@ -20631,8 +20737,8 @@
         <v>60</v>
       </c>
       <c r="N48" s="239"/>
-      <c r="O48" s="269"/>
-      <c r="P48" s="270"/>
+      <c r="O48" s="272"/>
+      <c r="P48" s="273"/>
       <c r="Q48" s="247"/>
       <c r="R48" s="248"/>
       <c r="S48" s="248"/>
@@ -20640,8 +20746,8 @@
       <c r="U48" s="248"/>
       <c r="V48" s="249"/>
       <c r="W48" s="239"/>
-      <c r="X48" s="264"/>
-      <c r="Y48" s="265"/>
+      <c r="X48" s="267"/>
+      <c r="Y48" s="268"/>
     </row>
     <row r="49" spans="2:25" ht="42" customHeight="1">
       <c r="B49" s="241">
@@ -20652,12 +20758,12 @@
       </c>
       <c r="D49" s="243"/>
       <c r="E49" s="244"/>
-      <c r="F49" s="267"/>
-      <c r="G49" s="268"/>
-      <c r="H49" s="268"/>
-      <c r="I49" s="268"/>
-      <c r="J49" s="268"/>
-      <c r="K49" s="268"/>
+      <c r="F49" s="270"/>
+      <c r="G49" s="271"/>
+      <c r="H49" s="271"/>
+      <c r="I49" s="271"/>
+      <c r="J49" s="271"/>
+      <c r="K49" s="271"/>
       <c r="L49" s="245" t="s">
         <v>60</v>
       </c>
@@ -20665,8 +20771,8 @@
         <v>60</v>
       </c>
       <c r="N49" s="239"/>
-      <c r="O49" s="269"/>
-      <c r="P49" s="270"/>
+      <c r="O49" s="272"/>
+      <c r="P49" s="273"/>
       <c r="Q49" s="247"/>
       <c r="R49" s="248"/>
       <c r="S49" s="248"/>
@@ -20674,8 +20780,8 @@
       <c r="U49" s="248"/>
       <c r="V49" s="249"/>
       <c r="W49" s="239"/>
-      <c r="X49" s="264"/>
-      <c r="Y49" s="265"/>
+      <c r="X49" s="267"/>
+      <c r="Y49" s="268"/>
     </row>
     <row r="50" spans="2:25" ht="42" customHeight="1">
       <c r="B50" s="241">
@@ -20686,12 +20792,12 @@
       </c>
       <c r="D50" s="243"/>
       <c r="E50" s="244"/>
-      <c r="F50" s="267"/>
-      <c r="G50" s="268"/>
-      <c r="H50" s="268"/>
-      <c r="I50" s="268"/>
-      <c r="J50" s="268"/>
-      <c r="K50" s="268"/>
+      <c r="F50" s="270"/>
+      <c r="G50" s="271"/>
+      <c r="H50" s="271"/>
+      <c r="I50" s="271"/>
+      <c r="J50" s="271"/>
+      <c r="K50" s="271"/>
       <c r="L50" s="245" t="s">
         <v>60</v>
       </c>
@@ -20699,8 +20805,8 @@
         <v>60</v>
       </c>
       <c r="N50" s="239"/>
-      <c r="O50" s="269"/>
-      <c r="P50" s="270"/>
+      <c r="O50" s="272"/>
+      <c r="P50" s="273"/>
       <c r="Q50" s="247"/>
       <c r="R50" s="248"/>
       <c r="S50" s="248"/>
@@ -20708,8 +20814,8 @@
       <c r="U50" s="248"/>
       <c r="V50" s="249"/>
       <c r="W50" s="239"/>
-      <c r="X50" s="264"/>
-      <c r="Y50" s="265"/>
+      <c r="X50" s="267"/>
+      <c r="Y50" s="268"/>
     </row>
     <row r="51" spans="2:25" ht="42" customHeight="1">
       <c r="B51" s="241">
@@ -20720,12 +20826,12 @@
       </c>
       <c r="D51" s="243"/>
       <c r="E51" s="244"/>
-      <c r="F51" s="267"/>
-      <c r="G51" s="268"/>
-      <c r="H51" s="268"/>
-      <c r="I51" s="268"/>
-      <c r="J51" s="268"/>
-      <c r="K51" s="268"/>
+      <c r="F51" s="270"/>
+      <c r="G51" s="271"/>
+      <c r="H51" s="271"/>
+      <c r="I51" s="271"/>
+      <c r="J51" s="271"/>
+      <c r="K51" s="271"/>
       <c r="L51" s="245" t="s">
         <v>60</v>
       </c>
@@ -20733,8 +20839,8 @@
         <v>60</v>
       </c>
       <c r="N51" s="239"/>
-      <c r="O51" s="269"/>
-      <c r="P51" s="270"/>
+      <c r="O51" s="272"/>
+      <c r="P51" s="273"/>
       <c r="Q51" s="247"/>
       <c r="R51" s="248"/>
       <c r="S51" s="248"/>
@@ -20742,8 +20848,8 @@
       <c r="U51" s="248"/>
       <c r="V51" s="249"/>
       <c r="W51" s="239"/>
-      <c r="X51" s="264"/>
-      <c r="Y51" s="265"/>
+      <c r="X51" s="267"/>
+      <c r="Y51" s="268"/>
     </row>
     <row r="52" spans="2:25" ht="42" customHeight="1">
       <c r="B52" s="241">
@@ -20754,12 +20860,12 @@
       </c>
       <c r="D52" s="243"/>
       <c r="E52" s="244"/>
-      <c r="F52" s="267"/>
-      <c r="G52" s="268"/>
-      <c r="H52" s="268"/>
-      <c r="I52" s="268"/>
-      <c r="J52" s="268"/>
-      <c r="K52" s="268"/>
+      <c r="F52" s="270"/>
+      <c r="G52" s="271"/>
+      <c r="H52" s="271"/>
+      <c r="I52" s="271"/>
+      <c r="J52" s="271"/>
+      <c r="K52" s="271"/>
       <c r="L52" s="245" t="s">
         <v>60</v>
       </c>
@@ -20767,8 +20873,8 @@
         <v>60</v>
       </c>
       <c r="N52" s="239"/>
-      <c r="O52" s="269"/>
-      <c r="P52" s="270"/>
+      <c r="O52" s="272"/>
+      <c r="P52" s="273"/>
       <c r="Q52" s="247"/>
       <c r="R52" s="248"/>
       <c r="S52" s="248"/>
@@ -20776,8 +20882,8 @@
       <c r="U52" s="248"/>
       <c r="V52" s="249"/>
       <c r="W52" s="239"/>
-      <c r="X52" s="264"/>
-      <c r="Y52" s="265"/>
+      <c r="X52" s="267"/>
+      <c r="Y52" s="268"/>
     </row>
     <row r="53" spans="2:25" ht="42" customHeight="1">
       <c r="B53" s="241">
@@ -20788,12 +20894,12 @@
       </c>
       <c r="D53" s="243"/>
       <c r="E53" s="244"/>
-      <c r="F53" s="267"/>
-      <c r="G53" s="268"/>
-      <c r="H53" s="268"/>
-      <c r="I53" s="268"/>
-      <c r="J53" s="268"/>
-      <c r="K53" s="268"/>
+      <c r="F53" s="270"/>
+      <c r="G53" s="271"/>
+      <c r="H53" s="271"/>
+      <c r="I53" s="271"/>
+      <c r="J53" s="271"/>
+      <c r="K53" s="271"/>
       <c r="L53" s="245" t="s">
         <v>60</v>
       </c>
@@ -20801,8 +20907,8 @@
         <v>60</v>
       </c>
       <c r="N53" s="239"/>
-      <c r="O53" s="269"/>
-      <c r="P53" s="270"/>
+      <c r="O53" s="272"/>
+      <c r="P53" s="273"/>
       <c r="Q53" s="247"/>
       <c r="R53" s="248"/>
       <c r="S53" s="248"/>
@@ -20810,8 +20916,8 @@
       <c r="U53" s="248"/>
       <c r="V53" s="249"/>
       <c r="W53" s="239"/>
-      <c r="X53" s="264"/>
-      <c r="Y53" s="265"/>
+      <c r="X53" s="267"/>
+      <c r="Y53" s="268"/>
     </row>
     <row r="54" spans="2:25" ht="42" customHeight="1">
       <c r="B54" s="241">
@@ -20822,12 +20928,12 @@
       </c>
       <c r="D54" s="243"/>
       <c r="E54" s="244"/>
-      <c r="F54" s="267"/>
-      <c r="G54" s="268"/>
-      <c r="H54" s="268"/>
-      <c r="I54" s="268"/>
-      <c r="J54" s="268"/>
-      <c r="K54" s="268"/>
+      <c r="F54" s="270"/>
+      <c r="G54" s="271"/>
+      <c r="H54" s="271"/>
+      <c r="I54" s="271"/>
+      <c r="J54" s="271"/>
+      <c r="K54" s="271"/>
       <c r="L54" s="245" t="s">
         <v>60</v>
       </c>
@@ -20835,8 +20941,8 @@
         <v>60</v>
       </c>
       <c r="N54" s="239"/>
-      <c r="O54" s="269"/>
-      <c r="P54" s="270"/>
+      <c r="O54" s="272"/>
+      <c r="P54" s="273"/>
       <c r="Q54" s="247"/>
       <c r="R54" s="248"/>
       <c r="S54" s="248"/>
@@ -20844,8 +20950,8 @@
       <c r="U54" s="248"/>
       <c r="V54" s="249"/>
       <c r="W54" s="239"/>
-      <c r="X54" s="264"/>
-      <c r="Y54" s="265"/>
+      <c r="X54" s="267"/>
+      <c r="Y54" s="268"/>
     </row>
     <row r="55" spans="2:25" ht="42" customHeight="1">
       <c r="B55" s="241">
@@ -20856,12 +20962,12 @@
       </c>
       <c r="D55" s="243"/>
       <c r="E55" s="244"/>
-      <c r="F55" s="267"/>
-      <c r="G55" s="268"/>
-      <c r="H55" s="268"/>
-      <c r="I55" s="268"/>
-      <c r="J55" s="268"/>
-      <c r="K55" s="268"/>
+      <c r="F55" s="270"/>
+      <c r="G55" s="271"/>
+      <c r="H55" s="271"/>
+      <c r="I55" s="271"/>
+      <c r="J55" s="271"/>
+      <c r="K55" s="271"/>
       <c r="L55" s="245" t="s">
         <v>60</v>
       </c>
@@ -20869,8 +20975,8 @@
         <v>60</v>
       </c>
       <c r="N55" s="239"/>
-      <c r="O55" s="269"/>
-      <c r="P55" s="270"/>
+      <c r="O55" s="272"/>
+      <c r="P55" s="273"/>
       <c r="Q55" s="247"/>
       <c r="R55" s="248"/>
       <c r="S55" s="248"/>
@@ -20878,8 +20984,8 @@
       <c r="U55" s="248"/>
       <c r="V55" s="249"/>
       <c r="W55" s="239"/>
-      <c r="X55" s="264"/>
-      <c r="Y55" s="265"/>
+      <c r="X55" s="267"/>
+      <c r="Y55" s="268"/>
     </row>
     <row r="56" spans="2:25" ht="42" customHeight="1">
       <c r="B56" s="241">
@@ -20890,12 +20996,12 @@
       </c>
       <c r="D56" s="243"/>
       <c r="E56" s="244"/>
-      <c r="F56" s="267"/>
-      <c r="G56" s="268"/>
-      <c r="H56" s="268"/>
-      <c r="I56" s="268"/>
-      <c r="J56" s="268"/>
-      <c r="K56" s="268"/>
+      <c r="F56" s="270"/>
+      <c r="G56" s="271"/>
+      <c r="H56" s="271"/>
+      <c r="I56" s="271"/>
+      <c r="J56" s="271"/>
+      <c r="K56" s="271"/>
       <c r="L56" s="245" t="s">
         <v>60</v>
       </c>
@@ -20903,8 +21009,8 @@
         <v>60</v>
       </c>
       <c r="N56" s="239"/>
-      <c r="O56" s="269"/>
-      <c r="P56" s="270"/>
+      <c r="O56" s="272"/>
+      <c r="P56" s="273"/>
       <c r="Q56" s="247"/>
       <c r="R56" s="248"/>
       <c r="S56" s="248"/>
@@ -20912,8 +21018,8 @@
       <c r="U56" s="248"/>
       <c r="V56" s="249"/>
       <c r="W56" s="239"/>
-      <c r="X56" s="264"/>
-      <c r="Y56" s="265"/>
+      <c r="X56" s="267"/>
+      <c r="Y56" s="268"/>
     </row>
     <row r="57" spans="2:25" ht="42" customHeight="1">
       <c r="B57" s="241">
@@ -20924,12 +21030,12 @@
       </c>
       <c r="D57" s="243"/>
       <c r="E57" s="244"/>
-      <c r="F57" s="267"/>
-      <c r="G57" s="268"/>
-      <c r="H57" s="268"/>
-      <c r="I57" s="268"/>
-      <c r="J57" s="268"/>
-      <c r="K57" s="268"/>
+      <c r="F57" s="270"/>
+      <c r="G57" s="271"/>
+      <c r="H57" s="271"/>
+      <c r="I57" s="271"/>
+      <c r="J57" s="271"/>
+      <c r="K57" s="271"/>
       <c r="L57" s="245" t="s">
         <v>60</v>
       </c>
@@ -20937,8 +21043,8 @@
         <v>60</v>
       </c>
       <c r="N57" s="239"/>
-      <c r="O57" s="269"/>
-      <c r="P57" s="270"/>
+      <c r="O57" s="272"/>
+      <c r="P57" s="273"/>
       <c r="Q57" s="247"/>
       <c r="R57" s="248"/>
       <c r="S57" s="248"/>
@@ -20946,8 +21052,8 @@
       <c r="U57" s="248"/>
       <c r="V57" s="249"/>
       <c r="W57" s="239"/>
-      <c r="X57" s="264"/>
-      <c r="Y57" s="265"/>
+      <c r="X57" s="267"/>
+      <c r="Y57" s="268"/>
     </row>
     <row r="58" spans="2:25" ht="42" customHeight="1">
       <c r="B58" s="241">
@@ -20958,12 +21064,12 @@
       </c>
       <c r="D58" s="243"/>
       <c r="E58" s="244"/>
-      <c r="F58" s="267"/>
-      <c r="G58" s="268"/>
-      <c r="H58" s="268"/>
-      <c r="I58" s="268"/>
-      <c r="J58" s="268"/>
-      <c r="K58" s="268"/>
+      <c r="F58" s="270"/>
+      <c r="G58" s="271"/>
+      <c r="H58" s="271"/>
+      <c r="I58" s="271"/>
+      <c r="J58" s="271"/>
+      <c r="K58" s="271"/>
       <c r="L58" s="245" t="s">
         <v>60</v>
       </c>
@@ -20971,8 +21077,8 @@
         <v>60</v>
       </c>
       <c r="N58" s="239"/>
-      <c r="O58" s="269"/>
-      <c r="P58" s="270"/>
+      <c r="O58" s="272"/>
+      <c r="P58" s="273"/>
       <c r="Q58" s="247"/>
       <c r="R58" s="248"/>
       <c r="S58" s="248"/>
@@ -20980,8 +21086,8 @@
       <c r="U58" s="248"/>
       <c r="V58" s="249"/>
       <c r="W58" s="239"/>
-      <c r="X58" s="264"/>
-      <c r="Y58" s="265"/>
+      <c r="X58" s="267"/>
+      <c r="Y58" s="268"/>
     </row>
     <row r="59" spans="2:25" ht="42" customHeight="1">
       <c r="B59" s="241">
@@ -20992,12 +21098,12 @@
       </c>
       <c r="D59" s="243"/>
       <c r="E59" s="244"/>
-      <c r="F59" s="267"/>
-      <c r="G59" s="268"/>
-      <c r="H59" s="268"/>
-      <c r="I59" s="268"/>
-      <c r="J59" s="268"/>
-      <c r="K59" s="268"/>
+      <c r="F59" s="270"/>
+      <c r="G59" s="271"/>
+      <c r="H59" s="271"/>
+      <c r="I59" s="271"/>
+      <c r="J59" s="271"/>
+      <c r="K59" s="271"/>
       <c r="L59" s="245" t="s">
         <v>60</v>
       </c>
@@ -21005,8 +21111,8 @@
         <v>60</v>
       </c>
       <c r="N59" s="239"/>
-      <c r="O59" s="269"/>
-      <c r="P59" s="270"/>
+      <c r="O59" s="272"/>
+      <c r="P59" s="273"/>
       <c r="Q59" s="247"/>
       <c r="R59" s="248"/>
       <c r="S59" s="248"/>
@@ -21014,8 +21120,8 @@
       <c r="U59" s="248"/>
       <c r="V59" s="249"/>
       <c r="W59" s="239"/>
-      <c r="X59" s="264"/>
-      <c r="Y59" s="265"/>
+      <c r="X59" s="267"/>
+      <c r="Y59" s="268"/>
     </row>
     <row r="60" spans="2:25" ht="42" customHeight="1">
       <c r="B60" s="241">
@@ -21026,12 +21132,12 @@
       </c>
       <c r="D60" s="243"/>
       <c r="E60" s="244"/>
-      <c r="F60" s="267"/>
-      <c r="G60" s="268"/>
-      <c r="H60" s="268"/>
-      <c r="I60" s="268"/>
-      <c r="J60" s="268"/>
-      <c r="K60" s="268"/>
+      <c r="F60" s="270"/>
+      <c r="G60" s="271"/>
+      <c r="H60" s="271"/>
+      <c r="I60" s="271"/>
+      <c r="J60" s="271"/>
+      <c r="K60" s="271"/>
       <c r="L60" s="245" t="s">
         <v>60</v>
       </c>
@@ -21039,8 +21145,8 @@
         <v>60</v>
       </c>
       <c r="N60" s="239"/>
-      <c r="O60" s="269"/>
-      <c r="P60" s="270"/>
+      <c r="O60" s="272"/>
+      <c r="P60" s="273"/>
       <c r="Q60" s="247"/>
       <c r="R60" s="248"/>
       <c r="S60" s="248"/>
@@ -21048,8 +21154,8 @@
       <c r="U60" s="248"/>
       <c r="V60" s="249"/>
       <c r="W60" s="239"/>
-      <c r="X60" s="264"/>
-      <c r="Y60" s="265"/>
+      <c r="X60" s="267"/>
+      <c r="Y60" s="268"/>
     </row>
     <row r="61" spans="2:25" ht="42" customHeight="1">
       <c r="B61" s="241">
@@ -21060,12 +21166,12 @@
       </c>
       <c r="D61" s="243"/>
       <c r="E61" s="244"/>
-      <c r="F61" s="267"/>
-      <c r="G61" s="268"/>
-      <c r="H61" s="268"/>
-      <c r="I61" s="268"/>
-      <c r="J61" s="268"/>
-      <c r="K61" s="268"/>
+      <c r="F61" s="270"/>
+      <c r="G61" s="271"/>
+      <c r="H61" s="271"/>
+      <c r="I61" s="271"/>
+      <c r="J61" s="271"/>
+      <c r="K61" s="271"/>
       <c r="L61" s="245" t="s">
         <v>60</v>
       </c>
@@ -21073,8 +21179,8 @@
         <v>60</v>
       </c>
       <c r="N61" s="239"/>
-      <c r="O61" s="269"/>
-      <c r="P61" s="270"/>
+      <c r="O61" s="272"/>
+      <c r="P61" s="273"/>
       <c r="Q61" s="247"/>
       <c r="R61" s="248"/>
       <c r="S61" s="248"/>
@@ -21082,8 +21188,8 @@
       <c r="U61" s="248"/>
       <c r="V61" s="249"/>
       <c r="W61" s="239"/>
-      <c r="X61" s="264"/>
-      <c r="Y61" s="265"/>
+      <c r="X61" s="267"/>
+      <c r="Y61" s="268"/>
     </row>
     <row r="62" spans="2:25" ht="42" customHeight="1">
       <c r="B62" s="241">
@@ -21094,12 +21200,12 @@
       </c>
       <c r="D62" s="243"/>
       <c r="E62" s="244"/>
-      <c r="F62" s="267"/>
-      <c r="G62" s="268"/>
-      <c r="H62" s="268"/>
-      <c r="I62" s="268"/>
-      <c r="J62" s="268"/>
-      <c r="K62" s="268"/>
+      <c r="F62" s="270"/>
+      <c r="G62" s="271"/>
+      <c r="H62" s="271"/>
+      <c r="I62" s="271"/>
+      <c r="J62" s="271"/>
+      <c r="K62" s="271"/>
       <c r="L62" s="245" t="s">
         <v>60</v>
       </c>
@@ -21107,8 +21213,8 @@
         <v>60</v>
       </c>
       <c r="N62" s="239"/>
-      <c r="O62" s="269"/>
-      <c r="P62" s="270"/>
+      <c r="O62" s="272"/>
+      <c r="P62" s="273"/>
       <c r="Q62" s="247"/>
       <c r="R62" s="248"/>
       <c r="S62" s="248"/>
@@ -21116,8 +21222,8 @@
       <c r="U62" s="248"/>
       <c r="V62" s="249"/>
       <c r="W62" s="239"/>
-      <c r="X62" s="264"/>
-      <c r="Y62" s="265"/>
+      <c r="X62" s="267"/>
+      <c r="Y62" s="268"/>
     </row>
     <row r="63" spans="2:25" ht="42" customHeight="1">
       <c r="B63" s="241">
@@ -21128,12 +21234,12 @@
       </c>
       <c r="D63" s="243"/>
       <c r="E63" s="244"/>
-      <c r="F63" s="267"/>
-      <c r="G63" s="268"/>
-      <c r="H63" s="268"/>
-      <c r="I63" s="268"/>
-      <c r="J63" s="268"/>
-      <c r="K63" s="268"/>
+      <c r="F63" s="270"/>
+      <c r="G63" s="271"/>
+      <c r="H63" s="271"/>
+      <c r="I63" s="271"/>
+      <c r="J63" s="271"/>
+      <c r="K63" s="271"/>
       <c r="L63" s="245" t="s">
         <v>60</v>
       </c>
@@ -21141,8 +21247,8 @@
         <v>60</v>
       </c>
       <c r="N63" s="239"/>
-      <c r="O63" s="269"/>
-      <c r="P63" s="270"/>
+      <c r="O63" s="272"/>
+      <c r="P63" s="273"/>
       <c r="Q63" s="247"/>
       <c r="R63" s="248"/>
       <c r="S63" s="248"/>
@@ -21150,8 +21256,8 @@
       <c r="U63" s="248"/>
       <c r="V63" s="249"/>
       <c r="W63" s="239"/>
-      <c r="X63" s="264"/>
-      <c r="Y63" s="265"/>
+      <c r="X63" s="267"/>
+      <c r="Y63" s="268"/>
     </row>
     <row r="64" spans="2:25" ht="42" customHeight="1">
       <c r="B64" s="241">
@@ -21162,12 +21268,12 @@
       </c>
       <c r="D64" s="243"/>
       <c r="E64" s="244"/>
-      <c r="F64" s="267"/>
-      <c r="G64" s="268"/>
-      <c r="H64" s="268"/>
-      <c r="I64" s="268"/>
-      <c r="J64" s="268"/>
-      <c r="K64" s="268"/>
+      <c r="F64" s="270"/>
+      <c r="G64" s="271"/>
+      <c r="H64" s="271"/>
+      <c r="I64" s="271"/>
+      <c r="J64" s="271"/>
+      <c r="K64" s="271"/>
       <c r="L64" s="245" t="s">
         <v>60</v>
       </c>
@@ -21175,8 +21281,8 @@
         <v>60</v>
       </c>
       <c r="N64" s="239"/>
-      <c r="O64" s="269"/>
-      <c r="P64" s="270"/>
+      <c r="O64" s="272"/>
+      <c r="P64" s="273"/>
       <c r="Q64" s="247"/>
       <c r="R64" s="248"/>
       <c r="S64" s="248"/>
@@ -21184,8 +21290,8 @@
       <c r="U64" s="248"/>
       <c r="V64" s="249"/>
       <c r="W64" s="239"/>
-      <c r="X64" s="264"/>
-      <c r="Y64" s="265"/>
+      <c r="X64" s="267"/>
+      <c r="Y64" s="268"/>
     </row>
     <row r="65" spans="2:40" ht="42" customHeight="1">
       <c r="B65" s="241">
@@ -21196,12 +21302,12 @@
       </c>
       <c r="D65" s="243"/>
       <c r="E65" s="244"/>
-      <c r="F65" s="267"/>
-      <c r="G65" s="268"/>
-      <c r="H65" s="268"/>
-      <c r="I65" s="268"/>
-      <c r="J65" s="268"/>
-      <c r="K65" s="268"/>
+      <c r="F65" s="270"/>
+      <c r="G65" s="271"/>
+      <c r="H65" s="271"/>
+      <c r="I65" s="271"/>
+      <c r="J65" s="271"/>
+      <c r="K65" s="271"/>
       <c r="L65" s="245" t="s">
         <v>60</v>
       </c>
@@ -21209,8 +21315,8 @@
         <v>60</v>
       </c>
       <c r="N65" s="239"/>
-      <c r="O65" s="269"/>
-      <c r="P65" s="270"/>
+      <c r="O65" s="272"/>
+      <c r="P65" s="273"/>
       <c r="Q65" s="247"/>
       <c r="R65" s="248"/>
       <c r="S65" s="248"/>
@@ -21218,8 +21324,8 @@
       <c r="U65" s="248"/>
       <c r="V65" s="249"/>
       <c r="W65" s="239"/>
-      <c r="X65" s="264"/>
-      <c r="Y65" s="265"/>
+      <c r="X65" s="267"/>
+      <c r="Y65" s="268"/>
     </row>
     <row r="66" spans="2:40" ht="42" customHeight="1">
       <c r="B66" s="241">
@@ -21230,12 +21336,12 @@
       </c>
       <c r="D66" s="243"/>
       <c r="E66" s="244"/>
-      <c r="F66" s="267"/>
-      <c r="G66" s="268"/>
-      <c r="H66" s="268"/>
-      <c r="I66" s="268"/>
-      <c r="J66" s="268"/>
-      <c r="K66" s="268"/>
+      <c r="F66" s="270"/>
+      <c r="G66" s="271"/>
+      <c r="H66" s="271"/>
+      <c r="I66" s="271"/>
+      <c r="J66" s="271"/>
+      <c r="K66" s="271"/>
       <c r="L66" s="245" t="s">
         <v>60</v>
       </c>
@@ -21243,8 +21349,8 @@
         <v>60</v>
       </c>
       <c r="N66" s="239"/>
-      <c r="O66" s="269"/>
-      <c r="P66" s="270"/>
+      <c r="O66" s="272"/>
+      <c r="P66" s="273"/>
       <c r="Q66" s="247"/>
       <c r="R66" s="248"/>
       <c r="S66" s="248"/>
@@ -21252,8 +21358,8 @@
       <c r="U66" s="248"/>
       <c r="V66" s="249"/>
       <c r="W66" s="239"/>
-      <c r="X66" s="264"/>
-      <c r="Y66" s="265"/>
+      <c r="X66" s="267"/>
+      <c r="Y66" s="268"/>
     </row>
     <row r="67" spans="2:40" ht="42" customHeight="1">
       <c r="B67" s="241">
@@ -21264,12 +21370,12 @@
       </c>
       <c r="D67" s="243"/>
       <c r="E67" s="244"/>
-      <c r="F67" s="267"/>
-      <c r="G67" s="268"/>
-      <c r="H67" s="268"/>
-      <c r="I67" s="268"/>
-      <c r="J67" s="268"/>
-      <c r="K67" s="268"/>
+      <c r="F67" s="270"/>
+      <c r="G67" s="271"/>
+      <c r="H67" s="271"/>
+      <c r="I67" s="271"/>
+      <c r="J67" s="271"/>
+      <c r="K67" s="271"/>
       <c r="L67" s="245" t="s">
         <v>60</v>
       </c>
@@ -21277,8 +21383,8 @@
         <v>60</v>
       </c>
       <c r="N67" s="239"/>
-      <c r="O67" s="269"/>
-      <c r="P67" s="270"/>
+      <c r="O67" s="272"/>
+      <c r="P67" s="273"/>
       <c r="Q67" s="247"/>
       <c r="R67" s="248"/>
       <c r="S67" s="248"/>
@@ -21286,8 +21392,8 @@
       <c r="U67" s="248"/>
       <c r="V67" s="249"/>
       <c r="W67" s="239"/>
-      <c r="X67" s="264"/>
-      <c r="Y67" s="265"/>
+      <c r="X67" s="267"/>
+      <c r="Y67" s="268"/>
     </row>
     <row r="68" spans="2:40" ht="42" customHeight="1">
       <c r="B68" s="241">
@@ -21298,12 +21404,12 @@
       </c>
       <c r="D68" s="243"/>
       <c r="E68" s="244"/>
-      <c r="F68" s="267"/>
-      <c r="G68" s="268"/>
-      <c r="H68" s="268"/>
-      <c r="I68" s="268"/>
-      <c r="J68" s="268"/>
-      <c r="K68" s="268"/>
+      <c r="F68" s="270"/>
+      <c r="G68" s="271"/>
+      <c r="H68" s="271"/>
+      <c r="I68" s="271"/>
+      <c r="J68" s="271"/>
+      <c r="K68" s="271"/>
       <c r="L68" s="245" t="s">
         <v>60</v>
       </c>
@@ -21311,8 +21417,8 @@
         <v>60</v>
       </c>
       <c r="N68" s="239"/>
-      <c r="O68" s="269"/>
-      <c r="P68" s="270"/>
+      <c r="O68" s="272"/>
+      <c r="P68" s="273"/>
       <c r="Q68" s="247"/>
       <c r="R68" s="248"/>
       <c r="S68" s="248"/>
@@ -21320,8 +21426,8 @@
       <c r="U68" s="248"/>
       <c r="V68" s="249"/>
       <c r="W68" s="239"/>
-      <c r="X68" s="264"/>
-      <c r="Y68" s="265"/>
+      <c r="X68" s="267"/>
+      <c r="Y68" s="268"/>
     </row>
     <row r="69" spans="2:40" ht="42" customHeight="1">
       <c r="B69" s="241">
@@ -21332,12 +21438,12 @@
       </c>
       <c r="D69" s="243"/>
       <c r="E69" s="244"/>
-      <c r="F69" s="267"/>
-      <c r="G69" s="268"/>
-      <c r="H69" s="268"/>
-      <c r="I69" s="268"/>
-      <c r="J69" s="268"/>
-      <c r="K69" s="268"/>
+      <c r="F69" s="270"/>
+      <c r="G69" s="271"/>
+      <c r="H69" s="271"/>
+      <c r="I69" s="271"/>
+      <c r="J69" s="271"/>
+      <c r="K69" s="271"/>
       <c r="L69" s="245" t="s">
         <v>60</v>
       </c>
@@ -21345,8 +21451,8 @@
         <v>60</v>
       </c>
       <c r="N69" s="239"/>
-      <c r="O69" s="269"/>
-      <c r="P69" s="270"/>
+      <c r="O69" s="272"/>
+      <c r="P69" s="273"/>
       <c r="Q69" s="247"/>
       <c r="R69" s="248"/>
       <c r="S69" s="248"/>
@@ -21354,8 +21460,8 @@
       <c r="U69" s="248"/>
       <c r="V69" s="249"/>
       <c r="W69" s="239"/>
-      <c r="X69" s="264"/>
-      <c r="Y69" s="265"/>
+      <c r="X69" s="267"/>
+      <c r="Y69" s="268"/>
     </row>
     <row r="70" spans="2:40" ht="42" customHeight="1">
       <c r="B70" s="241">
@@ -21366,12 +21472,12 @@
       </c>
       <c r="D70" s="243"/>
       <c r="E70" s="244"/>
-      <c r="F70" s="267"/>
-      <c r="G70" s="268"/>
-      <c r="H70" s="268"/>
-      <c r="I70" s="268"/>
-      <c r="J70" s="268"/>
-      <c r="K70" s="268"/>
+      <c r="F70" s="270"/>
+      <c r="G70" s="271"/>
+      <c r="H70" s="271"/>
+      <c r="I70" s="271"/>
+      <c r="J70" s="271"/>
+      <c r="K70" s="271"/>
       <c r="L70" s="245" t="s">
         <v>60</v>
       </c>
@@ -21379,8 +21485,8 @@
         <v>60</v>
       </c>
       <c r="N70" s="239"/>
-      <c r="O70" s="269"/>
-      <c r="P70" s="270"/>
+      <c r="O70" s="272"/>
+      <c r="P70" s="273"/>
       <c r="Q70" s="247"/>
       <c r="R70" s="248"/>
       <c r="S70" s="248"/>
@@ -21388,8 +21494,8 @@
       <c r="U70" s="248"/>
       <c r="V70" s="249"/>
       <c r="W70" s="239"/>
-      <c r="X70" s="264"/>
-      <c r="Y70" s="265"/>
+      <c r="X70" s="267"/>
+      <c r="Y70" s="268"/>
     </row>
     <row r="71" spans="2:40" ht="42" customHeight="1">
       <c r="B71" s="241">
@@ -21400,12 +21506,12 @@
       </c>
       <c r="D71" s="243"/>
       <c r="E71" s="244"/>
-      <c r="F71" s="267"/>
-      <c r="G71" s="268"/>
-      <c r="H71" s="268"/>
-      <c r="I71" s="268"/>
-      <c r="J71" s="268"/>
-      <c r="K71" s="268"/>
+      <c r="F71" s="270"/>
+      <c r="G71" s="271"/>
+      <c r="H71" s="271"/>
+      <c r="I71" s="271"/>
+      <c r="J71" s="271"/>
+      <c r="K71" s="271"/>
       <c r="L71" s="245" t="s">
         <v>60</v>
       </c>
@@ -21413,8 +21519,8 @@
         <v>60</v>
       </c>
       <c r="N71" s="239"/>
-      <c r="O71" s="269"/>
-      <c r="P71" s="270"/>
+      <c r="O71" s="272"/>
+      <c r="P71" s="273"/>
       <c r="Q71" s="247"/>
       <c r="R71" s="248"/>
       <c r="S71" s="248"/>
@@ -21422,8 +21528,8 @@
       <c r="U71" s="248"/>
       <c r="V71" s="249"/>
       <c r="W71" s="239"/>
-      <c r="X71" s="264"/>
-      <c r="Y71" s="265"/>
+      <c r="X71" s="267"/>
+      <c r="Y71" s="268"/>
     </row>
     <row r="72" spans="2:40" ht="42" customHeight="1" thickBot="1">
       <c r="B72" s="241">
@@ -21434,12 +21540,12 @@
       </c>
       <c r="D72" s="243"/>
       <c r="E72" s="244"/>
-      <c r="F72" s="267"/>
-      <c r="G72" s="268"/>
-      <c r="H72" s="268"/>
-      <c r="I72" s="268"/>
-      <c r="J72" s="268"/>
-      <c r="K72" s="268"/>
+      <c r="F72" s="270"/>
+      <c r="G72" s="271"/>
+      <c r="H72" s="271"/>
+      <c r="I72" s="271"/>
+      <c r="J72" s="271"/>
+      <c r="K72" s="271"/>
       <c r="L72" s="245" t="s">
         <v>60</v>
       </c>
@@ -21447,8 +21553,8 @@
         <v>60</v>
       </c>
       <c r="N72" s="239"/>
-      <c r="O72" s="269"/>
-      <c r="P72" s="270"/>
+      <c r="O72" s="272"/>
+      <c r="P72" s="273"/>
       <c r="Q72" s="247"/>
       <c r="R72" s="252"/>
       <c r="S72" s="252"/>
@@ -21468,12 +21574,12 @@
       </c>
       <c r="D73" s="243"/>
       <c r="E73" s="244"/>
-      <c r="F73" s="267"/>
-      <c r="G73" s="268"/>
-      <c r="H73" s="268"/>
-      <c r="I73" s="268"/>
-      <c r="J73" s="268"/>
-      <c r="K73" s="268"/>
+      <c r="F73" s="270"/>
+      <c r="G73" s="271"/>
+      <c r="H73" s="271"/>
+      <c r="I73" s="271"/>
+      <c r="J73" s="271"/>
+      <c r="K73" s="271"/>
       <c r="L73" s="245" t="s">
         <v>60</v>
       </c>
@@ -21481,8 +21587,8 @@
         <v>60</v>
       </c>
       <c r="N73" s="239"/>
-      <c r="O73" s="269"/>
-      <c r="P73" s="270"/>
+      <c r="O73" s="272"/>
+      <c r="P73" s="273"/>
       <c r="Q73" s="247"/>
       <c r="R73" s="256"/>
       <c r="S73" s="256"/>
@@ -21502,12 +21608,12 @@
       </c>
       <c r="D74" s="243"/>
       <c r="E74" s="244"/>
-      <c r="F74" s="267"/>
-      <c r="G74" s="268"/>
-      <c r="H74" s="268"/>
-      <c r="I74" s="268"/>
-      <c r="J74" s="268"/>
-      <c r="K74" s="268"/>
+      <c r="F74" s="270"/>
+      <c r="G74" s="271"/>
+      <c r="H74" s="271"/>
+      <c r="I74" s="271"/>
+      <c r="J74" s="271"/>
+      <c r="K74" s="271"/>
       <c r="L74" s="245" t="s">
         <v>60</v>
       </c>
@@ -21515,8 +21621,8 @@
         <v>60</v>
       </c>
       <c r="N74" s="239"/>
-      <c r="O74" s="269"/>
-      <c r="P74" s="270"/>
+      <c r="O74" s="272"/>
+      <c r="P74" s="273"/>
       <c r="Q74" s="247"/>
       <c r="R74" s="258"/>
       <c r="S74" s="258"/>
@@ -21536,12 +21642,12 @@
       </c>
       <c r="D75" s="243"/>
       <c r="E75" s="244"/>
-      <c r="F75" s="267"/>
-      <c r="G75" s="268"/>
-      <c r="H75" s="268"/>
-      <c r="I75" s="268"/>
-      <c r="J75" s="268"/>
-      <c r="K75" s="268"/>
+      <c r="F75" s="270"/>
+      <c r="G75" s="271"/>
+      <c r="H75" s="271"/>
+      <c r="I75" s="271"/>
+      <c r="J75" s="271"/>
+      <c r="K75" s="271"/>
       <c r="L75" s="245" t="s">
         <v>60</v>
       </c>
@@ -21549,8 +21655,8 @@
         <v>60</v>
       </c>
       <c r="N75" s="239"/>
-      <c r="O75" s="269"/>
-      <c r="P75" s="270"/>
+      <c r="O75" s="272"/>
+      <c r="P75" s="273"/>
       <c r="Q75" s="247"/>
       <c r="R75" s="260"/>
       <c r="S75" s="260"/>
@@ -21570,12 +21676,12 @@
       </c>
       <c r="D76" s="243"/>
       <c r="E76" s="244"/>
-      <c r="F76" s="267"/>
-      <c r="G76" s="268"/>
-      <c r="H76" s="268"/>
-      <c r="I76" s="268"/>
-      <c r="J76" s="268"/>
-      <c r="K76" s="268"/>
+      <c r="F76" s="270"/>
+      <c r="G76" s="271"/>
+      <c r="H76" s="271"/>
+      <c r="I76" s="271"/>
+      <c r="J76" s="271"/>
+      <c r="K76" s="271"/>
       <c r="L76" s="245" t="s">
         <v>60</v>
       </c>
@@ -21583,8 +21689,8 @@
         <v>60</v>
       </c>
       <c r="N76" s="239"/>
-      <c r="O76" s="269"/>
-      <c r="P76" s="270"/>
+      <c r="O76" s="272"/>
+      <c r="P76" s="273"/>
       <c r="Q76" s="247"/>
       <c r="R76" s="262"/>
       <c r="S76" s="262"/>
@@ -21615,7 +21721,11 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="254">
+  <mergeCells count="260">
+    <mergeCell ref="Q38:V38"/>
+    <mergeCell ref="Q39:V39"/>
+    <mergeCell ref="Q40:V40"/>
+    <mergeCell ref="Q41:V41"/>
     <mergeCell ref="F76:K76"/>
     <mergeCell ref="O76:P76"/>
     <mergeCell ref="X71:Y71"/>
@@ -21751,13 +21861,6 @@
     <mergeCell ref="X38:Y38"/>
     <mergeCell ref="F37:K37"/>
     <mergeCell ref="X28:Y28"/>
-    <mergeCell ref="F36:K36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="X26:Y26"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="U23:W23"/>
     <mergeCell ref="U25:W25"/>
     <mergeCell ref="O31:P31"/>
     <mergeCell ref="X31:Y31"/>
@@ -21770,11 +21873,25 @@
     <mergeCell ref="O34:P34"/>
     <mergeCell ref="F33:K33"/>
     <mergeCell ref="O33:P33"/>
-    <mergeCell ref="X37:Y37"/>
-    <mergeCell ref="X36:Y36"/>
     <mergeCell ref="F31:K31"/>
     <mergeCell ref="Q29:V29"/>
     <mergeCell ref="Q31:V31"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:K27"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:K23"/>
+    <mergeCell ref="F36:K36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F29:K29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="R16:T16"/>
     <mergeCell ref="X40:Y40"/>
     <mergeCell ref="X21:Y21"/>
     <mergeCell ref="B25:C25"/>
@@ -21792,14 +21909,6 @@
     <mergeCell ref="D24:K24"/>
     <mergeCell ref="L24:Q24"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D22:K22"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:K27"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:K23"/>
-    <mergeCell ref="Q30:V30"/>
     <mergeCell ref="R23:T23"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="U17:W17"/>
@@ -21812,27 +21921,10 @@
     <mergeCell ref="J5:O6"/>
     <mergeCell ref="J8:O8"/>
     <mergeCell ref="J10:O10"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F29:K29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="H17:Q17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D22:K22"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="U23:W23"/>
     <mergeCell ref="U18:W18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="F19:G19"/>
@@ -21843,6 +21935,19 @@
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="L16:M16"/>
     <mergeCell ref="N16:O16"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="D20:K20"/>
+    <mergeCell ref="L20:Q20"/>
+    <mergeCell ref="R18:T18"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:Y1"/>
     <mergeCell ref="G3:I3"/>
@@ -21858,6 +21963,13 @@
     <mergeCell ref="W8:Y12"/>
     <mergeCell ref="T3:Y3"/>
     <mergeCell ref="T8:V12"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="H17:Q17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="Q36:V36"/>
+    <mergeCell ref="Q37:V37"/>
     <mergeCell ref="X29:Y29"/>
     <mergeCell ref="N26:N27"/>
     <mergeCell ref="O26:P27"/>
@@ -21866,10 +21978,10 @@
     <mergeCell ref="L26:M27"/>
     <mergeCell ref="Q26:V27"/>
     <mergeCell ref="Q28:V28"/>
-    <mergeCell ref="X18:Y18"/>
-    <mergeCell ref="D20:K20"/>
-    <mergeCell ref="L20:Q20"/>
-    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="Q30:V30"/>
+    <mergeCell ref="X26:Y26"/>
+    <mergeCell ref="X37:Y37"/>
+    <mergeCell ref="X36:Y36"/>
   </mergeCells>
   <phoneticPr fontId="6"/>
   <conditionalFormatting sqref="H16:I16 L16:M16 P16:Q16 H17 F18">
@@ -21878,25 +21990,25 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN77" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN77">
       <formula1>"(Select from list),$J$120,$J$121,$J$122,$J$123,$J$125"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X17:Y25" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X17:Y25">
       <formula1>"(Select from list),Line,Page,Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M28:M76" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M28:M76">
       <formula1>"(Select from list),Defect,Risk,Problem,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:C76" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:C76">
       <formula1>"(Select from list),①,②,③,④,⑤,⑥,⑦,⑧,⑨,⑩"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L28:L76" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L28:L76">
       <formula1>"(Select from list),Issue,Question"</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0">
     <oddFooter>&amp;C&amp;9&amp;P/&amp;N</oddFooter>
   </headerFooter>
@@ -21904,7 +22016,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
     <pageSetUpPr fitToPage="1"/>
@@ -26589,25 +26701,25 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:M17" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:M17">
       <formula1>"(Select from list),Yes (Attached to this template), Yes (project)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X24:Y33" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X24:Y33">
       <formula1>"(Select from list),Line,Page,Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M39:M88" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M39:M88">
       <formula1>"(Select from list),Defect,Risk,Problem,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C39:C88" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C39:C88">
       <formula1>"(Select from list),①,②,③,④,⑤,⑥,⑦,⑧,⑨,⑩"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L39:L88" xr:uid="{00000000-0002-0000-0100-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L39:L88">
       <formula1>"(Select from list),Issue,Question"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J113:Y113" xr:uid="{00000000-0002-0000-0100-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J113:Y113">
       <formula1>"(Select from list),A,B,C,D,E,F"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T106:Y107" xr:uid="{00000000-0002-0000-0100-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T106:Y107">
       <formula1>" (Select from list),A,B"</formula1>
     </dataValidation>
   </dataValidations>
@@ -26644,7 +26756,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
     <pageSetUpPr fitToPage="1"/>
@@ -31092,25 +31204,25 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:M17" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:M17">
       <formula1>"(Select from list),Yes (Attached to this template), Yes (project)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X24:Y33" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X24:Y33">
       <formula1>"(Select from list),Line,Page,Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M39:M88" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M39:M88">
       <formula1>"(Select from list),Defect,Risk,Problem,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C39:C88" xr:uid="{00000000-0002-0000-0200-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C39:C88">
       <formula1>"(Select from list),①,②,③,④,⑤,⑥,⑦,⑧,⑨,⑩"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L39:L88" xr:uid="{00000000-0002-0000-0200-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L39:L88">
       <formula1>"(Select from list),Issue,Question"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J112:Y112" xr:uid="{00000000-0002-0000-0200-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J112:Y112">
       <formula1>"(Select from list),A,B,C,D,E,F"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T106:Y106" xr:uid="{00000000-0002-0000-0200-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T106:Y106">
       <formula1>" (Select from list),A,B"</formula1>
     </dataValidation>
   </dataValidations>
@@ -31128,7 +31240,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H171"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
@@ -33827,7 +33939,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E10 E15:E20 E155:E158 E91:E96 E123 E146:E150 E163:E170 E42:E52 E27 E25 E34:E37 E39:E40 E29:E31 E57 E59 E61:E63 E139 E71:E72 E74:E83 E85:E89 E102:E112 E114 E116:E118 E120:E121 E128:E129 E141:E144 E133:E135 E131 E137 E65:E69" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E10 E15:E20 E155:E158 E91:E96 E123 E146:E150 E163:E170 E42:E52 E27 E25 E34:E37 E39:E40 E29:E31 E57 E59 E61:E63 E139 E71:E72 E74:E83 E85:E89 E102:E112 E114 E116:E118 E120:E121 E128:E129 E141:E144 E133:E135 E131 E137 E65:E69">
       <formula1>"(Select from list),○,×,N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -33851,7 +33963,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>